<commit_message>
Double check analyses and names
</commit_message>
<xml_diff>
--- a/Supplementary_Morphology_Stats.xlsx
+++ b/Supplementary_Morphology_Stats.xlsx
@@ -8,22 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/185965a385c69db2/Documents/Moquegua_Morphology/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_45CD47DCE9434D1592334D05230B6DABE5749311" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_864007211D8A0FAADAD7533633DFC5002F0F9B39" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C472F810-5C30-4C87-8B6F-7FFA2BFE069E}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Welch_ANOVA" sheetId="1" r:id="rId1"/>
     <sheet name="Games_Howell" sheetId="2" r:id="rId2"/>
     <sheet name="MANOVA_Pillai" sheetId="3" r:id="rId3"/>
     <sheet name="Univariate_ANOVAs" sheetId="4" r:id="rId4"/>
+    <sheet name="Summary_Stats" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="54">
   <si>
     <t>Df</t>
   </si>
@@ -73,27 +74,36 @@
     <t>Diameter_mm</t>
   </si>
   <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>Length_mm</t>
+  </si>
+  <si>
+    <t>***</t>
+  </si>
+  <si>
+    <t>Mean_cupule_height(mm)</t>
+  </si>
+  <si>
+    <t>Mean_Cupule_Width(mm)</t>
+  </si>
+  <si>
+    <t>**</t>
+  </si>
+  <si>
+    <t>Mean_kernel_row</t>
+  </si>
+  <si>
+    <t>ns</t>
+  </si>
+  <si>
+    <t>Total_Wt_g</t>
+  </si>
+  <si>
     <t>****</t>
   </si>
   <si>
-    <t>Length_mm</t>
-  </si>
-  <si>
-    <t>Mean_cupule_height(mm)</t>
-  </si>
-  <si>
-    <t>Mean_Cupule_Width(mm)</t>
-  </si>
-  <si>
-    <t>Mean_kernel_row</t>
-  </si>
-  <si>
-    <t>Total_Wt_g</t>
-  </si>
-  <si>
-    <t>ns</t>
-  </si>
-  <si>
     <t>Pillai</t>
   </si>
   <si>
@@ -158,6 +168,24 @@
   </si>
   <si>
     <t xml:space="preserve"> Response Total_Wt_g</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Missing</t>
+  </si>
+  <si>
+    <t>Mean</t>
+  </si>
+  <si>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>Max</t>
   </si>
 </sst>
 </file>
@@ -221,6 +249,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -535,10 +567,10 @@
         <v>6</v>
       </c>
       <c r="B2">
-        <v>740.36020073155487</v>
+        <v>26.106120753073139</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>2.9643297449151121E-14</v>
       </c>
       <c r="D2" t="s">
         <v>4</v>
@@ -553,9 +585,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="3" width="23.26953125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
@@ -594,16 +629,16 @@
         <v>15</v>
       </c>
       <c r="D2">
-        <v>5.6705469663505266</v>
+        <v>6.1560000000000006</v>
       </c>
       <c r="E2">
-        <v>4.6565142866942626</v>
+        <v>0.98182371634237686</v>
       </c>
       <c r="F2">
-        <v>6.6845796460067897</v>
+        <v>11.330176283657631</v>
       </c>
       <c r="G2">
-        <v>1.6200000000000001E-10</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="H2" t="s">
         <v>16</v>
@@ -620,19 +655,19 @@
         <v>17</v>
       </c>
       <c r="D3">
-        <v>34.79141288813824</v>
+        <v>42.655999999999999</v>
       </c>
       <c r="E3">
-        <v>31.324154504494611</v>
+        <v>16.60118885351428</v>
       </c>
       <c r="F3">
-        <v>38.258671271781871</v>
+        <v>68.710811146485725</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>5.44E-4</v>
       </c>
       <c r="H3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
@@ -643,22 +678,22 @@
         <v>14</v>
       </c>
       <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4">
+        <v>-5.4269337016999986</v>
+      </c>
+      <c r="E4">
+        <v>-8.8007447603884437</v>
+      </c>
+      <c r="F4">
+        <v>-2.0531226430115539</v>
+      </c>
+      <c r="G4">
+        <v>7.5199999999999996E-4</v>
+      </c>
+      <c r="H4" t="s">
         <v>18</v>
-      </c>
-      <c r="D4">
-        <v>-4.9771520367220994</v>
-      </c>
-      <c r="E4">
-        <v>-5.4247208989740923</v>
-      </c>
-      <c r="F4">
-        <v>-4.5295831744701056</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
@@ -669,22 +704,22 @@
         <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D5">
-        <v>-3.675089215836624</v>
+        <v>-4.5462707182000006</v>
       </c>
       <c r="E5">
-        <v>-4.1580604551417508</v>
+        <v>-8.0397386362285364</v>
       </c>
       <c r="F5">
-        <v>-3.1921179765314971</v>
+        <v>-1.0528028001714651</v>
       </c>
       <c r="G5">
-        <v>1.9200000000000001E-10</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="H5" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
@@ -695,22 +730,22 @@
         <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D6">
-        <v>4.6096531116745476</v>
+        <v>5.4666666665000001</v>
       </c>
       <c r="E6">
-        <v>3.5489813668426202</v>
+        <v>-1.6540043377690019</v>
       </c>
       <c r="F6">
-        <v>5.6703248565064772</v>
+        <v>12.587337670768999</v>
       </c>
       <c r="G6">
-        <v>9.6000000000000005E-11</v>
+        <v>0.221</v>
       </c>
       <c r="H6" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
@@ -721,22 +756,22 @@
         <v>14</v>
       </c>
       <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7">
+        <v>-5.7285000000000004</v>
+      </c>
+      <c r="E7">
+        <v>-9.9418496201076891</v>
+      </c>
+      <c r="F7">
+        <v>-1.515150379892312</v>
+      </c>
+      <c r="G7">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="H7" t="s">
         <v>21</v>
-      </c>
-      <c r="D7">
-        <v>-6.1788105755489147</v>
-      </c>
-      <c r="E7">
-        <v>-6.7063499622016156</v>
-      </c>
-      <c r="F7">
-        <v>-5.6512711888962137</v>
-      </c>
-      <c r="G7">
-        <v>1.7399999999999999E-10</v>
-      </c>
-      <c r="H7" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
@@ -750,19 +785,19 @@
         <v>17</v>
       </c>
       <c r="D8">
-        <v>29.120865921787711</v>
+        <v>36.5</v>
       </c>
       <c r="E8">
-        <v>25.561635490876419</v>
+        <v>10.357860605650281</v>
       </c>
       <c r="F8">
-        <v>32.680096352699003</v>
+        <v>62.642139394349719</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="H8" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
@@ -773,22 +808,22 @@
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D9">
-        <v>-10.64769900307263</v>
+        <v>-11.5829337017</v>
       </c>
       <c r="E9">
-        <v>-11.575242008106811</v>
+        <v>-15.926765660983611</v>
       </c>
       <c r="F9">
-        <v>-9.7201559980384395</v>
+        <v>-7.2391017424163886</v>
       </c>
       <c r="G9">
-        <v>0</v>
+        <v>5.9999999999999997E-7</v>
       </c>
       <c r="H9" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
@@ -799,22 +834,22 @@
         <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D10">
-        <v>-9.3456361821871496</v>
+        <v>-10.702270718199999</v>
       </c>
       <c r="E10">
-        <v>-10.290697538682331</v>
+        <v>-15.139248752568751</v>
       </c>
       <c r="F10">
-        <v>-8.400574825691967</v>
+        <v>-6.2652926838312526</v>
       </c>
       <c r="G10">
-        <v>0</v>
+        <v>1.4899999999999999E-6</v>
       </c>
       <c r="H10" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
@@ -825,22 +860,22 @@
         <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D11">
-        <v>-1.0608938546759781</v>
+        <v>-0.68933333350000048</v>
       </c>
       <c r="E11">
-        <v>-2.394497152463801</v>
+        <v>-8.2160798444996477</v>
       </c>
       <c r="F11">
-        <v>0.27270944311184508</v>
+        <v>6.8374131774996467</v>
       </c>
       <c r="G11">
-        <v>0.221</v>
+        <v>1</v>
       </c>
       <c r="H11" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
@@ -851,22 +886,22 @@
         <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D12">
-        <v>-11.84935754189944</v>
+        <v>-11.884499999999999</v>
       </c>
       <c r="E12">
-        <v>-12.817783989947189</v>
+        <v>-16.87466334801838</v>
       </c>
       <c r="F12">
-        <v>-10.880931093851689</v>
+        <v>-6.8943366519816189</v>
       </c>
       <c r="G12">
-        <v>0</v>
+        <v>2.5199999999999998E-7</v>
       </c>
       <c r="H12" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
@@ -877,22 +912,22 @@
         <v>17</v>
       </c>
       <c r="C13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13">
+        <v>-48.0829337017</v>
+      </c>
+      <c r="E13">
+        <v>-74.02197175690813</v>
+      </c>
+      <c r="F13">
+        <v>-22.14389564649187</v>
+      </c>
+      <c r="G13">
+        <v>1.2899999999999999E-4</v>
+      </c>
+      <c r="H13" t="s">
         <v>18</v>
-      </c>
-      <c r="D13">
-        <v>-39.768564924860343</v>
-      </c>
-      <c r="E13">
-        <v>-43.211625926232117</v>
-      </c>
-      <c r="F13">
-        <v>-36.325503923488547</v>
-      </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-      <c r="H13" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
@@ -903,22 +938,22 @@
         <v>17</v>
       </c>
       <c r="C14" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D14">
-        <v>-38.466502103974861</v>
+        <v>-47.202270718199998</v>
       </c>
       <c r="E14">
-        <v>-41.914316438659533</v>
+        <v>-73.155743412478884</v>
       </c>
       <c r="F14">
-        <v>-35.018687769290189</v>
+        <v>-21.248798023921111</v>
       </c>
       <c r="G14">
-        <v>0</v>
+        <v>1.6200000000000001E-4</v>
       </c>
       <c r="H14" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
@@ -929,22 +964,22 @@
         <v>17</v>
       </c>
       <c r="C15" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D15">
-        <v>-30.181759776463689</v>
+        <v>-37.189333333500002</v>
       </c>
       <c r="E15">
-        <v>-33.754299095799468</v>
+        <v>-63.619304773657589</v>
       </c>
       <c r="F15">
-        <v>-26.609220457127901</v>
+        <v>-10.759361893342421</v>
       </c>
       <c r="G15">
-        <v>0</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="H15" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
@@ -955,22 +990,22 @@
         <v>17</v>
       </c>
       <c r="C16" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D16">
-        <v>-40.970223463687148</v>
+        <v>-48.384500000000003</v>
       </c>
       <c r="E16">
-        <v>-44.424494536446623</v>
+        <v>-74.415237274835448</v>
       </c>
       <c r="F16">
-        <v>-37.515952390927673</v>
+        <v>-22.35376272516455</v>
       </c>
       <c r="G16">
-        <v>0</v>
+        <v>1.16E-4</v>
       </c>
       <c r="H16" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
@@ -978,25 +1013,25 @@
         <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C17" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D17">
-        <v>1.302062820885475</v>
+        <v>0.88066298349999972</v>
       </c>
       <c r="E17">
-        <v>1.051565101851325</v>
+        <v>-0.53351370090204098</v>
       </c>
       <c r="F17">
-        <v>1.5525605399196249</v>
+        <v>2.29483966790204</v>
       </c>
       <c r="G17">
-        <v>4.4700000000000001E-10</v>
+        <v>0.45</v>
       </c>
       <c r="H17" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
@@ -1004,25 +1039,25 @@
         <v>13</v>
       </c>
       <c r="B18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18">
+        <v>10.8936003682</v>
+      </c>
+      <c r="E18">
+        <v>4.2867202235143136</v>
+      </c>
+      <c r="F18">
+        <v>17.500480512885691</v>
+      </c>
+      <c r="G18">
+        <v>5.13E-4</v>
+      </c>
+      <c r="H18" t="s">
         <v>18</v>
-      </c>
-      <c r="C18" t="s">
-        <v>20</v>
-      </c>
-      <c r="D18">
-        <v>9.5868051483966479</v>
-      </c>
-      <c r="E18">
-        <v>8.6084570043300577</v>
-      </c>
-      <c r="F18">
-        <v>10.56515329246324</v>
-      </c>
-      <c r="G18">
-        <v>0</v>
-      </c>
-      <c r="H18" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
@@ -1030,25 +1065,25 @@
         <v>13</v>
       </c>
       <c r="B19" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C19" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D19">
-        <v>-1.2016585388268159</v>
+        <v>-0.30156629829999998</v>
       </c>
       <c r="E19">
-        <v>-1.5307666912405611</v>
+        <v>-3.2960789182628161</v>
       </c>
       <c r="F19">
-        <v>-0.87255038641307059</v>
+        <v>2.692946321662816</v>
       </c>
       <c r="G19">
-        <v>1.43E-11</v>
+        <v>1</v>
       </c>
       <c r="H19" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
@@ -1056,25 +1091,25 @@
         <v>13</v>
       </c>
       <c r="B20" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C20" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D20">
-        <v>8.2847423275111716</v>
+        <v>10.012937384700001</v>
       </c>
       <c r="E20">
-        <v>7.2897726091068948</v>
+        <v>3.3473228863564768</v>
       </c>
       <c r="F20">
-        <v>9.2797120459154492</v>
+        <v>16.678551883043529</v>
       </c>
       <c r="G20">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="H20" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
@@ -1082,25 +1117,25 @@
         <v>13</v>
       </c>
       <c r="B21" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D21">
-        <v>-2.5037213597122912</v>
+        <v>-1.1822292818</v>
       </c>
       <c r="E21">
-        <v>-2.8797448260721419</v>
+        <v>-4.3203313356446298</v>
       </c>
       <c r="F21">
-        <v>-2.1276978933524391</v>
+        <v>1.9558727720446301</v>
       </c>
       <c r="G21">
-        <v>0</v>
+        <v>0.88800000000000001</v>
       </c>
       <c r="H21" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
@@ -1108,25 +1143,25 @@
         <v>13</v>
       </c>
       <c r="B22" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C22" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D22">
-        <v>-10.78846368722346</v>
+        <v>-11.1951666665</v>
       </c>
       <c r="E22">
-        <v>-11.805645695953549</v>
+        <v>-18.201367058897748</v>
       </c>
       <c r="F22">
-        <v>-9.7712816784933771</v>
+        <v>-4.1889662741022491</v>
       </c>
       <c r="G22">
-        <v>0</v>
+        <v>4.5399999999999998E-4</v>
       </c>
       <c r="H22" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1147,53 +1182,53 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B2">
-        <v>0.78328765570337422</v>
+        <v>0.70823186731958854</v>
       </c>
       <c r="C2">
-        <v>4.1957030485497722</v>
+        <v>4.713652636047355</v>
       </c>
       <c r="D2">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="E2">
-        <v>2331</v>
+        <v>2345</v>
       </c>
       <c r="F2">
-        <v>5.2145153342975567E-27</v>
+        <v>7.7069120129407653E-27</v>
       </c>
       <c r="G2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="G3" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1205,311 +1240,513 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B2">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C2">
-        <v>15274.03471703293</v>
+        <v>13008.07465881174</v>
       </c>
       <c r="D2">
-        <v>1527.403471703293</v>
+        <v>1626.009332351467</v>
       </c>
       <c r="E2">
-        <v>3.3524615325603642</v>
+        <v>3.5374899869692982</v>
       </c>
       <c r="F2">
-        <v>3.5384857470590399E-4</v>
+        <v>6.0072299842498357E-4</v>
       </c>
       <c r="G2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B3">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="C3">
-        <v>151716.98500854851</v>
+        <v>153982.94506676981</v>
       </c>
       <c r="D3">
-        <v>455.60656158723282</v>
+        <v>459.65058228886511</v>
       </c>
       <c r="G3" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B4">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C4">
-        <v>770.23485232860412</v>
+        <v>733.21052272583347</v>
       </c>
       <c r="D4">
-        <v>77.023485232860409</v>
+        <v>91.651315340729184</v>
       </c>
       <c r="E4">
-        <v>2.299415352094988</v>
+        <v>2.7434332656432261</v>
       </c>
       <c r="F4">
-        <v>1.2751237243106081E-2</v>
+        <v>6.0493770019202277E-3</v>
       </c>
       <c r="G4" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B5">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="C5">
-        <v>11154.496537206291</v>
+        <v>11191.52086680906</v>
       </c>
       <c r="D5">
-        <v>33.49698659821707</v>
+        <v>33.407524975549428</v>
       </c>
       <c r="G5" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B6">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C6">
-        <v>1003.175350843531</v>
+        <v>999.60464465473069</v>
       </c>
       <c r="D6">
-        <v>100.3175350843531</v>
+        <v>124.95058058184129</v>
       </c>
       <c r="E6">
-        <v>22.41664937261918</v>
+        <v>28.02162604019232</v>
       </c>
       <c r="F6">
-        <v>5.5672917049725489E-32</v>
+        <v>2.891178454484114E-33</v>
       </c>
       <c r="G6" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B7">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="C7">
-        <v>1490.21999799368</v>
+        <v>1493.790704182474</v>
       </c>
       <c r="D7">
-        <v>4.4751351291101491</v>
+        <v>4.4590767289029092</v>
       </c>
       <c r="G7" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B8">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C8">
-        <v>77.098206938475428</v>
+        <v>74.943363596209764</v>
       </c>
       <c r="D8">
-        <v>7.7098206938475426</v>
+        <v>9.3679204495262205</v>
       </c>
       <c r="E8">
-        <v>4.3212521600243479</v>
+        <v>5.2630415901031666</v>
       </c>
       <c r="F8">
-        <v>1.078247106113199E-5</v>
+        <v>3.1874077990861172E-6</v>
       </c>
       <c r="G8" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B9">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="C9">
-        <v>594.12646982322042</v>
+        <v>596.28131316548604</v>
       </c>
       <c r="D9">
-        <v>1.7841635730427039</v>
+        <v>1.7799442184044361</v>
       </c>
       <c r="G9" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B10">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C10">
-        <v>16.350401347994119</v>
+        <v>15.789613552776411</v>
       </c>
       <c r="D10">
-        <v>1.635040134799411</v>
+        <v>1.973701694097052</v>
       </c>
       <c r="E10">
-        <v>3.013755256795152</v>
+        <v>3.6485109233919668</v>
       </c>
       <c r="F10">
-        <v>1.1590824493206339E-3</v>
+        <v>4.3171743376798098E-4</v>
       </c>
       <c r="G10" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B11">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="C11">
-        <v>180.66110831680319</v>
+        <v>181.2218961120208</v>
       </c>
       <c r="D11">
-        <v>0.54252585080121074</v>
+        <v>0.54096088391648012</v>
       </c>
       <c r="G11" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B12">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C12">
-        <v>1673.186097456771</v>
+        <v>1230.6690769134029</v>
       </c>
       <c r="D12">
-        <v>167.31860974567709</v>
+        <v>153.83363461417539</v>
       </c>
       <c r="E12">
-        <v>4.7524878206497272</v>
+        <v>4.2358237226338993</v>
       </c>
       <c r="F12">
-        <v>2.219126743077242E-6</v>
+        <v>7.3715240698486893E-5</v>
       </c>
       <c r="G12" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B13">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="C13">
-        <v>11723.774820256809</v>
+        <v>12166.291840800201</v>
       </c>
       <c r="D13">
-        <v>35.206530991762207</v>
+        <v>36.317289077015531</v>
       </c>
       <c r="G13" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B14">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C14">
-        <v>64.18445937412838</v>
+        <v>63.146945331538099</v>
       </c>
       <c r="D14">
-        <v>6.4184459374128382</v>
+        <v>7.8933681664422624</v>
       </c>
       <c r="E14">
-        <v>1.685722986832233</v>
+        <v>2.083838330803883</v>
       </c>
       <c r="F14">
-        <v>8.2705568751329991E-2</v>
+        <v>3.6824532239004663E-2</v>
       </c>
       <c r="G14" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B15">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="C15">
-        <v>1267.908496149129</v>
+        <v>1268.946010191718</v>
       </c>
       <c r="D15">
-        <v>3.8075330214688572</v>
+        <v>3.7878985378857259</v>
       </c>
       <c r="G15" t="s">
-        <v>44</v>
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="23.26953125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2">
+        <v>344</v>
+      </c>
+      <c r="C2">
+        <v>14</v>
+      </c>
+      <c r="D2">
+        <v>7.7674418604651159</v>
+      </c>
+      <c r="E2">
+        <v>2.6961777009056109</v>
+      </c>
+      <c r="F2">
+        <v>4</v>
+      </c>
+      <c r="G2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3">
+        <v>358</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>13.437988826815641</v>
+      </c>
+      <c r="E3">
+        <v>5.8687688218627807</v>
+      </c>
+      <c r="F3">
+        <v>0.05</v>
+      </c>
+      <c r="G3">
+        <v>84.18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4">
+        <v>358</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>42.558854748603352</v>
+      </c>
+      <c r="E4">
+        <v>21.956453453701421</v>
+      </c>
+      <c r="F4">
+        <v>7.9</v>
+      </c>
+      <c r="G4">
+        <v>146.94999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5">
+        <v>358</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>4.0923526446284919</v>
+      </c>
+      <c r="E5">
+        <v>1.401801967930477</v>
+      </c>
+      <c r="F5">
+        <v>1.123388582</v>
+      </c>
+      <c r="G5">
+        <v>9.2909760590000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6">
+        <v>358</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>2.7902898237430169</v>
+      </c>
+      <c r="E6">
+        <v>0.77481505630577541</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7">
+        <v>358</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>12.377094972139661</v>
+      </c>
+      <c r="E7">
+        <v>6.195558523116639</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8">
+        <v>358</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>1.588631284916201</v>
+      </c>
+      <c r="E8">
+        <v>1.954876563641432</v>
+      </c>
+      <c r="F8">
+        <v>0.08</v>
+      </c>
+      <c r="G8">
+        <v>16.53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>